<commit_message>
Creacion de codigo con medidas de tendencia central
</commit_message>
<xml_diff>
--- a/Tabla-Comparativa/Tabla comparativa.xlsx
+++ b/Tabla-Comparativa/Tabla comparativa.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a7e664fa1e8d7ff2/Documentos/Uni David/Organizador/Analisis-NBA/Tabla-Comparativa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{E5B06131-81C8-498E-B803-B3BEDC8AB01E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB0B6B99-91DF-4229-9089-13D4E7295955}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="8_{483C549F-E6D5-4602-801A-0EF546EB6BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{150AF330-591F-4429-9229-70A218D15059}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13056" xr2:uid="{638C395F-4F58-42E5-9DFC-3943DCF5DAC1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabla comparativa" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="94">
   <si>
     <t xml:space="preserve">Duelo </t>
   </si>
@@ -297,14 +297,43 @@
   </si>
   <si>
     <t>Lakers vs Clippers</t>
+  </si>
+  <si>
+    <t>Rockets</t>
+  </si>
+  <si>
+    <t>Warriors</t>
+  </si>
+  <si>
+    <t>Spurs vs Grizzlies</t>
+  </si>
+  <si>
+    <t>Pistons vs Nets</t>
+  </si>
+  <si>
+    <t>Kings vs Rockets</t>
+  </si>
+  <si>
+    <t>76ers vs Warrios</t>
+  </si>
+  <si>
+    <t>Bucks vs Mavericks</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -332,12 +361,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -672,10 +702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B91AA06-A905-4D9A-85B2-F3BC00162813}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:XFD31"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="83" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -723,7 +753,7 @@
         <v>110</v>
       </c>
       <c r="F2">
-        <f>D2-E2</f>
+        <f t="shared" ref="F2:F9" si="0">D2-E2</f>
         <v>32</v>
       </c>
       <c r="G2" s="2">
@@ -747,7 +777,7 @@
         <v>99</v>
       </c>
       <c r="F3">
-        <f>D3-E3</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G3" s="2">
@@ -771,7 +801,7 @@
         <v>86</v>
       </c>
       <c r="F4">
-        <f>D4-E4</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="G4" s="2">
@@ -795,7 +825,7 @@
         <v>112</v>
       </c>
       <c r="F5">
-        <f>D5-E5</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G5" s="2">
@@ -819,7 +849,7 @@
         <v>97</v>
       </c>
       <c r="F6">
-        <f>D6-E6</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="G6" s="2">
@@ -843,7 +873,7 @@
         <v>116</v>
       </c>
       <c r="F7">
-        <f>D7-E7</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="G7" s="2">
@@ -867,7 +897,7 @@
         <v>128</v>
       </c>
       <c r="F8">
-        <f>D8-E8</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G8" s="2">
@@ -891,7 +921,7 @@
         <v>88</v>
       </c>
       <c r="F9">
-        <f>D9-E9</f>
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="G9" s="2">
@@ -915,7 +945,7 @@
         <v>101</v>
       </c>
       <c r="F10">
-        <f t="shared" ref="F10:F40" si="0">D10-E10</f>
+        <f t="shared" ref="F10:F46" si="1">D10-E10</f>
         <v>10</v>
       </c>
       <c r="G10" s="2">
@@ -939,7 +969,7 @@
         <v>103</v>
       </c>
       <c r="F11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="G11" s="2">
@@ -963,7 +993,7 @@
         <v>97</v>
       </c>
       <c r="F12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="G12" s="2">
@@ -987,7 +1017,7 @@
         <v>92</v>
       </c>
       <c r="F13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="G13" s="2">
@@ -1011,7 +1041,7 @@
         <v>82</v>
       </c>
       <c r="F14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="G14" s="2">
@@ -1035,7 +1065,7 @@
         <v>148</v>
       </c>
       <c r="F15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="G15" s="2">
@@ -1059,7 +1089,7 @@
         <v>99</v>
       </c>
       <c r="F16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="G16" s="2">
@@ -1083,7 +1113,7 @@
         <v>105</v>
       </c>
       <c r="F17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="G17" s="2">
@@ -1107,7 +1137,7 @@
         <v>121</v>
       </c>
       <c r="F18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="G18" s="2">
@@ -1131,7 +1161,7 @@
         <v>109</v>
       </c>
       <c r="F19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="G19" s="2">
@@ -1155,7 +1185,7 @@
         <v>117</v>
       </c>
       <c r="F20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="G20" s="2">
@@ -1179,7 +1209,7 @@
         <v>106</v>
       </c>
       <c r="F21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="G21" s="2">
@@ -1203,7 +1233,7 @@
         <v>91</v>
       </c>
       <c r="F22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="G22" s="2">
@@ -1227,7 +1257,7 @@
         <v>97</v>
       </c>
       <c r="F23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="G23" s="2">
@@ -1251,7 +1281,7 @@
         <v>121</v>
       </c>
       <c r="F24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="G24" s="2">
@@ -1275,7 +1305,7 @@
         <v>101</v>
       </c>
       <c r="F25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="G25" s="2">
@@ -1299,7 +1329,7 @@
         <v>115</v>
       </c>
       <c r="F26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="G26" s="2">
@@ -1323,7 +1353,7 @@
         <v>96</v>
       </c>
       <c r="F27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="G27" s="2">
@@ -1347,7 +1377,7 @@
         <v>102</v>
       </c>
       <c r="F28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G28" s="2">
@@ -1371,7 +1401,7 @@
         <v>112</v>
       </c>
       <c r="F29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G29" s="2">
@@ -1395,7 +1425,7 @@
         <v>116</v>
       </c>
       <c r="F30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="G30" s="2">
@@ -1419,7 +1449,7 @@
         <v>119</v>
       </c>
       <c r="F31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="G31" s="2">
@@ -1443,7 +1473,7 @@
         <v>119</v>
       </c>
       <c r="F32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="G32" s="2">
@@ -1467,7 +1497,7 @@
         <v>116</v>
       </c>
       <c r="F33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="G33" s="2">
@@ -1491,7 +1521,7 @@
         <v>102</v>
       </c>
       <c r="F34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="G34" s="2">
@@ -1515,7 +1545,7 @@
         <v>113</v>
       </c>
       <c r="F35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G35" s="2">
@@ -1539,7 +1569,7 @@
         <v>115</v>
       </c>
       <c r="F36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="G36" s="2">
@@ -1563,7 +1593,7 @@
         <v>120</v>
       </c>
       <c r="F37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="G37" s="2">
@@ -1587,7 +1617,7 @@
         <v>108</v>
       </c>
       <c r="F38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="G38" s="2">
@@ -1611,7 +1641,7 @@
         <v>116</v>
       </c>
       <c r="F39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G39" s="2">
@@ -1635,12 +1665,159 @@
         <v>102</v>
       </c>
       <c r="F40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="G40" s="2">
         <v>45716</v>
       </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" t="s">
+        <v>27</v>
+      </c>
+      <c r="D41">
+        <v>113</v>
+      </c>
+      <c r="E41">
+        <v>110</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="G41" s="2">
+        <v>45717</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>89</v>
+      </c>
+      <c r="B42" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42" t="s">
+        <v>41</v>
+      </c>
+      <c r="D42">
+        <v>130</v>
+      </c>
+      <c r="E42">
+        <v>128</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G42" s="2">
+        <v>45717</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>93</v>
+      </c>
+      <c r="B43" t="s">
+        <v>54</v>
+      </c>
+      <c r="C43" t="s">
+        <v>44</v>
+      </c>
+      <c r="D43">
+        <v>132</v>
+      </c>
+      <c r="E43">
+        <v>117</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="G43" s="2">
+        <v>45717</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>90</v>
+      </c>
+      <c r="B44" t="s">
+        <v>20</v>
+      </c>
+      <c r="C44" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44">
+        <v>115</v>
+      </c>
+      <c r="E44">
+        <v>94</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="G44" s="2">
+        <v>45717</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>91</v>
+      </c>
+      <c r="B45" t="s">
+        <v>26</v>
+      </c>
+      <c r="C45" t="s">
+        <v>87</v>
+      </c>
+      <c r="D45">
+        <v>113</v>
+      </c>
+      <c r="E45">
+        <v>103</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G45" s="2">
+        <v>45717</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>92</v>
+      </c>
+      <c r="B46" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" t="s">
+        <v>88</v>
+      </c>
+      <c r="D46">
+        <v>126</v>
+      </c>
+      <c r="E46">
+        <v>119</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="G46" s="2">
+        <v>45717</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D49" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>